<commit_message>
cleaning and max code
</commit_message>
<xml_diff>
--- a/data/out/standings_euro_fifa.xlsx
+++ b/data/out/standings_euro_fifa.xlsx
@@ -522,7 +522,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['Denmark', 'France', 'Belgium']</t>
+          <t>['Belgium', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -571,7 +571,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['Spain', 'Portugal', 'West Germany']</t>
+          <t>['Spain', 'West Germany', 'Portugal']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -620,7 +620,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain', 'West Germany']</t>
+          <t>['Spain', 'West Germany', 'Italy']</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -669,7 +669,7 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Republic of Ireland', 'Soviet Union']</t>
+          <t>['Netherlands', 'Soviet Union', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -718,7 +718,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['Denmark', 'France', 'Sweden']</t>
+          <t>['Sweden', 'Denmark', 'France']</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -767,7 +767,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Germany', 'CIS']</t>
+          <t>['Germany', 'CIS', 'Netherlands']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -875,7 +875,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['England', 'Scotland']</t>
+          <t>['Scotland', 'England']</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['England', 'Netherlands']</t>
+          <t>['Netherlands', 'England']</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1327,7 +1327,7 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Germany']</t>
+          <t>['Germany', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>['Italy', 'Germany']</t>
+          <t>['Germany', 'Italy']</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1494,7 +1494,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>['Croatia', 'Portugal']</t>
+          <t>['Portugal', 'Croatia']</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1769,7 +1769,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>['Italy', 'Turkey']</t>
+          <t>['Turkey', 'Italy']</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1877,7 +1877,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>['FR Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'FR Yugoslavia']</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>['FR Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'FR Yugoslavia']</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>['FR Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'FR Yugoslavia']</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>['FR Yugoslavia', 'Spain']</t>
+          <t>['Spain', 'FR Yugoslavia']</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2329,7 +2329,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>['Greece', 'Spain']</t>
+          <t>['Spain', 'Greece']</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2496,7 +2496,7 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2663,7 +2663,7 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>['Denmark', 'Sweden']</t>
+          <t>['Sweden', 'Denmark']</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2820,7 +2820,7 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>['Czech Republic', 'Portugal']</t>
+          <t>['Portugal', 'Czech Republic']</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2928,7 +2928,7 @@
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>['Croatia', 'Germany']</t>
+          <t>['Germany', 'Croatia']</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>['Italy', 'Netherlands']</t>
+          <t>['Netherlands', 'Italy']</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3085,7 +3085,7 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>['Russia', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Russia']</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3360,7 +3360,7 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>['Denmark', 'Germany']</t>
+          <t>['Germany', 'Denmark']</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3576,7 +3576,7 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>['England', 'France']</t>
+          <t>['France', 'England']</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -3625,7 +3625,7 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>['Switzerland', 'France']</t>
+          <t>['France', 'Switzerland']</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -3674,7 +3674,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>['England', 'Slovakia']</t>
+          <t>['Slovakia', 'England']</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>['England', 'Wales']</t>
+          <t>['Wales', 'England']</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -3880,7 +3880,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>['Italy', 'Belgium']</t>
+          <t>['Belgium', 'Italy']</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['Hungary', 'Portugal']</t>
+          <t>['Portugal', 'Hungary']</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -4096,7 +4096,7 @@
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr">
         <is>
-          <t>['Italy', 'Wales']</t>
+          <t>['Wales', 'Italy']</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -4145,7 +4145,7 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr">
         <is>
-          <t>['Finland', 'Belgium']</t>
+          <t>['Belgium', 'Finland']</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>['Denmark', 'Belgium']</t>
+          <t>['Belgium', 'Denmark']</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4469,7 +4469,7 @@
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Sweden']</t>
+          <t>['Sweden', 'Slovakia']</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -4528,7 +4528,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>['Spain', 'Sweden']</t>
+          <t>['Sweden', 'Spain']</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -4803,7 +4803,7 @@
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
         <is>
-          <t>['Switzerland', 'Germany']</t>
+          <t>['Germany', 'Switzerland']</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -4852,7 +4852,7 @@
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -4970,7 +4970,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>['Italy', 'Spain']</t>
+          <t>['Spain', 'Italy']</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -5019,7 +5019,7 @@
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
         <is>
-          <t>['England', 'Denmark']</t>
+          <t>['Denmark', 'England']</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -5137,7 +5137,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>['England', 'Denmark']</t>
+          <t>['Denmark', 'England']</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -5589,7 +5589,7 @@
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium']</t>
+          <t>['Belgium', 'Romania']</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>['Slovakia', 'Belgium']</t>
+          <t>['Belgium', 'Slovakia']</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -5707,7 +5707,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>['Romania', 'Belgium']</t>
+          <t>['Belgium', 'Romania']</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">

</xml_diff>